<commit_message>
Fixed missing cell borders
</commit_message>
<xml_diff>
--- a/ZSOX report template.xlsx
+++ b/ZSOX report template.xlsx
@@ -7,13 +7,13 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13200" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="4" r:id="rId1"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId2"/>
+    <sheet name="Arkusz3" sheetId="3" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="4" r:id="rId2"/>
     <sheet name="Arkusz2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="25" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -417,24 +417,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -451,6 +433,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -726,7 +726,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna1" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" showMissing="0" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" showMissing="0" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -1093,7 +1093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1101,53 +1101,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="27">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1164,20 +1120,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="19" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="20"/>
-      <c r="P1" s="21"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:18" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1230,24 +1186,24 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
@@ -1405,6 +1361,50 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="21">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>

</xml_diff>